<commit_message>
Cleaned up landing pages. Added frozen columns to combing. Added some calculations to calculate load on chart. Cleaned up some code, removed old code before dashboard. Added exporting of combing chart.
</commit_message>
<xml_diff>
--- a/IntelliTabler/timetable/static/excel_templates/combingTemplate.xlsx
+++ b/IntelliTabler/timetable/static/excel_templates/combingTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\Documents\intellitabler\IntelliTabler\timetable\static\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CA4656-7BA5-49AD-B9F4-B9465F98731F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534BD20C-4EFA-4634-84A4-D2C9854831CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="590" xr2:uid="{61D4E36C-3248-40E5-9387-ABEFDABC86B6}"/>
   </bookViews>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9082282A-69E5-475D-B57C-5460C13C5493}">
   <dimension ref="A1:DI40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="BA1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>